<commit_message>
Trying to restore order
</commit_message>
<xml_diff>
--- a/CompanyMatches.xlsx
+++ b/CompanyMatches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="25360" windowHeight="15380"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19983,14 +19983,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="38.33203125" customWidth="1"/>
-    <col min="4" max="4" width="62" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20525,7 +20525,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="409">
+    <row r="39" spans="1:4" ht="336">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -20553,7 +20553,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="409">
+    <row r="41" spans="1:4" ht="336">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="210">
+    <row r="42" spans="1:4" ht="42">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -20609,7 +20609,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="210">
+    <row r="45" spans="1:4" ht="42">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -20637,7 +20637,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="140">
+    <row r="47" spans="1:4" ht="28">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -20819,7 +20819,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="42">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -20959,7 +20959,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="409">
+    <row r="70" spans="1:4" ht="392">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -21015,7 +21015,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="409">
+    <row r="74" spans="1:4" ht="224">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -21127,7 +21127,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="409">
+    <row r="82" spans="1:4" ht="252">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -21169,7 +21169,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="409">
+    <row r="85" spans="1:4" ht="266">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -21211,7 +21211,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="154">
+    <row r="88" spans="1:4" ht="28">
       <c r="A88" t="s">
         <v>82</v>
       </c>
@@ -21337,7 +21337,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="350">
+    <row r="97" spans="1:4" ht="84">
       <c r="A97" t="s">
         <v>31</v>
       </c>
@@ -21365,7 +21365,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="409">
+    <row r="99" spans="1:4" ht="322">
       <c r="A99" t="s">
         <v>90</v>
       </c>
@@ -21393,7 +21393,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="409">
+    <row r="101" spans="1:4" ht="112">
       <c r="A101" t="s">
         <v>92</v>
       </c>
@@ -21519,7 +21519,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="154">
+    <row r="110" spans="1:4" ht="28">
       <c r="A110" t="s">
         <v>100</v>
       </c>
@@ -21533,7 +21533,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="409">
+    <row r="111" spans="1:4" ht="322">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -21589,7 +21589,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="409">
+    <row r="115" spans="1:4" ht="182">
       <c r="A115" t="s">
         <v>105</v>
       </c>
@@ -21603,7 +21603,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="210">
+    <row r="116" spans="1:4" ht="42">
       <c r="A116" t="s">
         <v>106</v>
       </c>
@@ -21645,7 +21645,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="409">
+    <row r="119" spans="1:4" ht="252">
       <c r="A119" t="s">
         <v>109</v>
       </c>
@@ -21659,7 +21659,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="409">
+    <row r="120" spans="1:4" ht="392">
       <c r="A120" t="s">
         <v>31</v>
       </c>
@@ -21701,7 +21701,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="350">
+    <row r="123" spans="1:4" ht="70">
       <c r="A123" t="s">
         <v>112</v>
       </c>
@@ -21715,7 +21715,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="409">
+    <row r="124" spans="1:4" ht="392">
       <c r="A124" t="s">
         <v>113</v>
       </c>
@@ -21757,7 +21757,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="210">
+    <row r="127" spans="1:4" ht="42">
       <c r="A127" t="s">
         <v>114</v>
       </c>
@@ -21785,7 +21785,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="224">
+    <row r="129" spans="1:4" ht="56">
       <c r="A129" t="s">
         <v>116</v>
       </c>
@@ -21813,7 +21813,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="56">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>118</v>
       </c>
@@ -21827,7 +21827,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="154">
+    <row r="132" spans="1:4" ht="28">
       <c r="A132" t="s">
         <v>119</v>
       </c>
@@ -21841,7 +21841,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="224">
+    <row r="133" spans="1:4" ht="56">
       <c r="A133" t="s">
         <v>120</v>
       </c>
@@ -21869,7 +21869,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="409">
+    <row r="135" spans="1:4" ht="252">
       <c r="A135" t="s">
         <v>79</v>
       </c>
@@ -21897,7 +21897,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="409">
+    <row r="137" spans="1:4" ht="294">
       <c r="A137" t="s">
         <v>122</v>
       </c>
@@ -21925,7 +21925,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="56">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>124</v>
       </c>
@@ -21939,7 +21939,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="70">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>32</v>
       </c>
@@ -21981,7 +21981,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="409">
+    <row r="143" spans="1:4" ht="336">
       <c r="A143" t="s">
         <v>127</v>
       </c>
@@ -22009,7 +22009,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="409">
+    <row r="145" spans="1:4" ht="322">
       <c r="A145" t="s">
         <v>129</v>
       </c>
@@ -22051,7 +22051,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="56">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>132</v>
       </c>
@@ -22065,7 +22065,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="70">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>133</v>
       </c>
@@ -22079,7 +22079,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="56">
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>79</v>
       </c>
@@ -22093,7 +22093,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="168">
+    <row r="151" spans="1:4" ht="42">
       <c r="A151" t="s">
         <v>134</v>
       </c>
@@ -22149,7 +22149,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="168">
+    <row r="155" spans="1:4" ht="42">
       <c r="A155" t="s">
         <v>138</v>
       </c>
@@ -22219,7 +22219,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="84">
+    <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>142</v>
       </c>
@@ -22317,7 +22317,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="409">
+    <row r="167" spans="1:4" ht="322">
       <c r="A167" t="s">
         <v>148</v>
       </c>
@@ -22373,7 +22373,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="56">
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
         <v>150</v>
       </c>
@@ -22415,7 +22415,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="409">
+    <row r="174" spans="1:4" ht="294">
       <c r="A174" t="s">
         <v>153</v>
       </c>
@@ -22443,7 +22443,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="409">
+    <row r="176" spans="1:4" ht="336">
       <c r="A176" t="s">
         <v>154</v>
       </c>
@@ -22471,7 +22471,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="112">
+    <row r="178" spans="1:4" ht="28">
       <c r="A178" t="s">
         <v>156</v>
       </c>
@@ -22513,7 +22513,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="210">
+    <row r="181" spans="1:4" ht="42">
       <c r="A181" t="s">
         <v>158</v>
       </c>
@@ -22527,7 +22527,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="409">
+    <row r="182" spans="1:4" ht="126">
       <c r="A182" t="s">
         <v>33</v>
       </c>
@@ -22583,7 +22583,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="409">
+    <row r="186" spans="1:4" ht="322">
       <c r="A186" t="s">
         <v>161</v>
       </c>
@@ -22597,7 +22597,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="409">
+    <row r="187" spans="1:4" ht="378">
       <c r="A187" t="s">
         <v>84</v>
       </c>
@@ -22625,7 +22625,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="154">
+    <row r="189" spans="1:4" ht="28">
       <c r="A189" t="s">
         <v>163</v>
       </c>
@@ -22681,7 +22681,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="409">
+    <row r="193" spans="1:4" ht="238">
       <c r="A193" t="s">
         <v>89</v>
       </c>
@@ -22723,7 +22723,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="210">
+    <row r="196" spans="1:4" ht="42">
       <c r="A196" t="s">
         <v>168</v>
       </c>
@@ -22793,7 +22793,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="409">
+    <row r="201" spans="1:4" ht="308">
       <c r="A201" t="s">
         <v>171</v>
       </c>
@@ -22821,7 +22821,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="409">
+    <row r="203" spans="1:4" ht="182">
       <c r="A203" t="s">
         <v>173</v>
       </c>
@@ -22919,7 +22919,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="409">
+    <row r="210" spans="1:4" ht="154">
       <c r="A210" t="s">
         <v>178</v>
       </c>
@@ -23045,7 +23045,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="409">
+    <row r="219" spans="1:4" ht="322">
       <c r="A219" t="s">
         <v>5</v>
       </c>
@@ -23101,7 +23101,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="409">
+    <row r="223" spans="1:4" ht="168">
       <c r="A223" t="s">
         <v>189</v>
       </c>
@@ -23143,7 +23143,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="56">
+    <row r="226" spans="1:4">
       <c r="A226" t="s">
         <v>192</v>
       </c>
@@ -23213,7 +23213,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="56">
+    <row r="231" spans="1:4">
       <c r="A231" t="s">
         <v>81</v>
       </c>
@@ -23255,7 +23255,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="154">
+    <row r="234" spans="1:4" ht="28">
       <c r="A234" t="s">
         <v>196</v>
       </c>
@@ -23311,7 +23311,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="42">
+    <row r="238" spans="1:4">
       <c r="A238" t="s">
         <v>59</v>
       </c>
@@ -23339,7 +23339,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="56">
+    <row r="240" spans="1:4">
       <c r="A240" t="s">
         <v>201</v>
       </c>
@@ -23381,7 +23381,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="154">
+    <row r="243" spans="1:4" ht="28">
       <c r="A243" t="s">
         <v>203</v>
       </c>
@@ -23437,7 +23437,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="210">
+    <row r="247" spans="1:4" ht="42">
       <c r="A247" t="s">
         <v>205</v>
       </c>
@@ -23451,7 +23451,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="409">
+    <row r="248" spans="1:4" ht="280">
       <c r="A248" t="s">
         <v>206</v>
       </c>
@@ -23479,7 +23479,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="210">
+    <row r="250" spans="1:4" ht="42">
       <c r="A250" t="s">
         <v>208</v>
       </c>
@@ -23703,7 +23703,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="210">
+    <row r="266" spans="1:4" ht="42">
       <c r="A266" t="s">
         <v>42</v>
       </c>
@@ -23801,7 +23801,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="210">
+    <row r="273" spans="1:4" ht="42">
       <c r="A273" t="s">
         <v>225</v>
       </c>
@@ -23815,7 +23815,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="154">
+    <row r="274" spans="1:4" ht="28">
       <c r="A274" t="s">
         <v>226</v>
       </c>
@@ -23829,7 +23829,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="409">
+    <row r="275" spans="1:4" ht="98">
       <c r="A275" t="s">
         <v>5</v>
       </c>
@@ -23857,7 +23857,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="409">
+    <row r="277" spans="1:4" ht="112">
       <c r="A277" t="s">
         <v>228</v>
       </c>
@@ -23899,7 +23899,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="409">
+    <row r="280" spans="1:4" ht="350">
       <c r="A280" t="s">
         <v>230</v>
       </c>
@@ -23969,7 +23969,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="409">
+    <row r="285" spans="1:4" ht="336">
       <c r="A285" t="s">
         <v>65</v>
       </c>
@@ -23997,7 +23997,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="409">
+    <row r="287" spans="1:4" ht="140">
       <c r="A287" t="s">
         <v>235</v>
       </c>
@@ -24025,7 +24025,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="70">
+    <row r="289" spans="1:4">
       <c r="A289" t="s">
         <v>237</v>
       </c>
@@ -24081,7 +24081,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="126">
+    <row r="293" spans="1:4" ht="28">
       <c r="A293" t="s">
         <v>241</v>
       </c>
@@ -24109,7 +24109,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="210">
+    <row r="295" spans="1:4" ht="42">
       <c r="A295" t="s">
         <v>243</v>
       </c>
@@ -24137,7 +24137,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="409">
+    <row r="297" spans="1:4" ht="336">
       <c r="A297" t="s">
         <v>245</v>
       </c>
@@ -24165,7 +24165,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="266">
+    <row r="299" spans="1:4" ht="70">
       <c r="A299" t="s">
         <v>247</v>
       </c>
@@ -24235,7 +24235,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="304" spans="1:4" ht="409">
+    <row r="304" spans="1:4" ht="322">
       <c r="A304" t="s">
         <v>191</v>
       </c>
@@ -24249,7 +24249,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="409">
+    <row r="305" spans="1:4" ht="392">
       <c r="A305" t="s">
         <v>251</v>
       </c>
@@ -24319,7 +24319,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="409">
+    <row r="310" spans="1:4" ht="252">
       <c r="A310" t="s">
         <v>207</v>
       </c>
@@ -24347,7 +24347,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="112">
+    <row r="312" spans="1:4" ht="28">
       <c r="A312" t="s">
         <v>257</v>
       </c>
@@ -24375,7 +24375,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="314" spans="1:4" ht="56">
+    <row r="314" spans="1:4">
       <c r="A314" t="s">
         <v>258</v>
       </c>
@@ -24403,7 +24403,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="210">
+    <row r="316" spans="1:4" ht="42">
       <c r="A316" t="s">
         <v>107</v>
       </c>
@@ -24473,7 +24473,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="321" spans="1:4" ht="409">
+    <row r="321" spans="1:4" ht="350">
       <c r="A321" t="s">
         <v>24</v>
       </c>
@@ -24515,7 +24515,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="324" spans="1:4" ht="409">
+    <row r="324" spans="1:4" ht="84">
       <c r="A324" t="s">
         <v>264</v>
       </c>
@@ -24557,7 +24557,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="327" spans="1:4" ht="154">
+    <row r="327" spans="1:4" ht="28">
       <c r="A327" t="s">
         <v>59</v>
       </c>
@@ -24669,7 +24669,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="335" spans="1:4" ht="210">
+    <row r="335" spans="1:4" ht="42">
       <c r="A335" t="s">
         <v>271</v>
       </c>
@@ -24711,7 +24711,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="338" spans="1:4" ht="140">
+    <row r="338" spans="1:4" ht="28">
       <c r="A338" t="s">
         <v>273</v>
       </c>
@@ -24725,7 +24725,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="339" spans="1:4" ht="56">
+    <row r="339" spans="1:4">
       <c r="A339" t="s">
         <v>274</v>
       </c>
@@ -24739,7 +24739,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="340" spans="1:4" ht="210">
+    <row r="340" spans="1:4" ht="42">
       <c r="A340" t="s">
         <v>89</v>
       </c>
@@ -24767,7 +24767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="342" spans="1:4" ht="56">
+    <row r="342" spans="1:4">
       <c r="A342" t="s">
         <v>276</v>
       </c>
@@ -24851,7 +24851,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="348" spans="1:4" ht="154">
+    <row r="348" spans="1:4" ht="28">
       <c r="A348" t="s">
         <v>40</v>
       </c>
@@ -24921,7 +24921,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="353" spans="1:4" ht="154">
+    <row r="353" spans="1:4" ht="28">
       <c r="A353" t="s">
         <v>284</v>
       </c>
@@ -24963,7 +24963,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="356" spans="1:4" ht="70">
+    <row r="356" spans="1:4">
       <c r="A356" t="s">
         <v>35</v>
       </c>
@@ -24991,7 +24991,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="358" spans="1:4" ht="409">
+    <row r="358" spans="1:4" ht="98">
       <c r="A358" t="s">
         <v>286</v>
       </c>
@@ -25005,7 +25005,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="359" spans="1:4" ht="42">
+    <row r="359" spans="1:4">
       <c r="A359" t="s">
         <v>287</v>
       </c>
@@ -25019,7 +25019,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="360" spans="1:4" ht="210">
+    <row r="360" spans="1:4" ht="42">
       <c r="A360" t="s">
         <v>288</v>
       </c>
@@ -25033,7 +25033,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="361" spans="1:4" ht="238">
+    <row r="361" spans="1:4" ht="56">
       <c r="A361" t="s">
         <v>289</v>
       </c>
@@ -25145,7 +25145,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="369" spans="1:4" ht="409">
+    <row r="369" spans="1:4" ht="252">
       <c r="A369" t="s">
         <v>295</v>
       </c>
@@ -25187,7 +25187,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="372" spans="1:4" ht="409">
+    <row r="372" spans="1:4" ht="266">
       <c r="A372" t="s">
         <v>107</v>
       </c>
@@ -25285,7 +25285,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="379" spans="1:4" ht="210">
+    <row r="379" spans="1:4" ht="42">
       <c r="A379" t="s">
         <v>303</v>
       </c>
@@ -25313,7 +25313,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="381" spans="1:4" ht="392">
+    <row r="381" spans="1:4" ht="70">
       <c r="A381" t="s">
         <v>305</v>
       </c>
@@ -25383,7 +25383,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="386" spans="1:4" ht="56">
+    <row r="386" spans="1:4">
       <c r="A386" t="s">
         <v>309</v>
       </c>
@@ -25397,7 +25397,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="387" spans="1:4" ht="409">
+    <row r="387" spans="1:4" ht="210">
       <c r="A387" t="s">
         <v>89</v>
       </c>
@@ -25411,7 +25411,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="388" spans="1:4" ht="70">
+    <row r="388" spans="1:4">
       <c r="A388" t="s">
         <v>35</v>
       </c>
@@ -25425,7 +25425,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="389" spans="1:4" ht="392">
+    <row r="389" spans="1:4" ht="70">
       <c r="A389" t="s">
         <v>310</v>
       </c>
@@ -25677,7 +25677,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="407" spans="1:4" ht="154">
+    <row r="407" spans="1:4" ht="28">
       <c r="A407" t="s">
         <v>321</v>
       </c>
@@ -25691,7 +25691,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="408" spans="1:4" ht="154">
+    <row r="408" spans="1:4" ht="28">
       <c r="A408" t="s">
         <v>322</v>
       </c>
@@ -25719,7 +25719,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="410" spans="1:4" ht="154">
+    <row r="410" spans="1:4" ht="28">
       <c r="A410" t="s">
         <v>323</v>
       </c>
@@ -25803,7 +25803,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="416" spans="1:4" ht="224">
+    <row r="416" spans="1:4" ht="56">
       <c r="A416" t="s">
         <v>227</v>
       </c>
@@ -25817,7 +25817,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="417" spans="1:4" ht="409">
+    <row r="417" spans="1:4" ht="364">
       <c r="A417" t="s">
         <v>326</v>
       </c>
@@ -25831,7 +25831,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="418" spans="1:4" ht="266">
+    <row r="418" spans="1:4" ht="56">
       <c r="A418" t="s">
         <v>327</v>
       </c>
@@ -25845,7 +25845,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="419" spans="1:4" ht="409">
+    <row r="419" spans="1:4" ht="308">
       <c r="A419" t="s">
         <v>84</v>
       </c>
@@ -25873,7 +25873,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="421" spans="1:4" ht="409">
+    <row r="421" spans="1:4" ht="322">
       <c r="A421" t="s">
         <v>328</v>
       </c>
@@ -25887,7 +25887,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="422" spans="1:4" ht="409">
+    <row r="422" spans="1:4" ht="182">
       <c r="A422" t="s">
         <v>118</v>
       </c>
@@ -25957,7 +25957,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="427" spans="1:4" ht="154">
+    <row r="427" spans="1:4" ht="28">
       <c r="A427" t="s">
         <v>306</v>
       </c>
@@ -25985,7 +25985,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="429" spans="1:4" ht="409">
+    <row r="429" spans="1:4" ht="406">
       <c r="A429" t="s">
         <v>334</v>
       </c>
@@ -26013,7 +26013,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="431" spans="1:4" ht="210">
+    <row r="431" spans="1:4" ht="42">
       <c r="A431" t="s">
         <v>335</v>
       </c>
@@ -26041,7 +26041,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="433" spans="1:4" ht="224">
+    <row r="433" spans="1:4" ht="56">
       <c r="A433" t="s">
         <v>336</v>
       </c>
@@ -26069,7 +26069,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="435" spans="1:4" ht="42">
+    <row r="435" spans="1:4">
       <c r="A435" t="s">
         <v>45</v>
       </c>
@@ -26083,7 +26083,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="436" spans="1:4" ht="409">
+    <row r="436" spans="1:4" ht="84">
       <c r="A436" t="s">
         <v>337</v>
       </c>
@@ -26139,7 +26139,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="440" spans="1:4" ht="409">
+    <row r="440" spans="1:4" ht="364">
       <c r="A440" t="s">
         <v>339</v>
       </c>
@@ -26153,7 +26153,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="441" spans="1:4" ht="392">
+    <row r="441" spans="1:4" ht="70">
       <c r="A441" t="s">
         <v>13</v>
       </c>
@@ -26209,7 +26209,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="445" spans="1:4" ht="210">
+    <row r="445" spans="1:4" ht="42">
       <c r="A445" t="s">
         <v>342</v>
       </c>
@@ -26251,7 +26251,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="448" spans="1:4" ht="409">
+    <row r="448" spans="1:4" ht="238">
       <c r="A448" t="s">
         <v>84</v>
       </c>
@@ -26279,7 +26279,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="450" spans="1:4" ht="409">
+    <row r="450" spans="1:4" ht="84">
       <c r="A450" t="s">
         <v>344</v>
       </c>
@@ -26293,7 +26293,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="451" spans="1:4" ht="409">
+    <row r="451" spans="1:4" ht="308">
       <c r="A451" t="s">
         <v>345</v>
       </c>
@@ -26475,7 +26475,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="464" spans="1:4" ht="70">
+    <row r="464" spans="1:4">
       <c r="A464" t="s">
         <v>79</v>
       </c>
@@ -26503,7 +26503,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="466" spans="1:4" ht="409">
+    <row r="466" spans="1:4" ht="84">
       <c r="A466" t="s">
         <v>353</v>
       </c>
@@ -26517,7 +26517,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="467" spans="1:4" ht="42">
+    <row r="467" spans="1:4">
       <c r="A467" t="s">
         <v>354</v>
       </c>
@@ -26531,7 +26531,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="468" spans="1:4" ht="210">
+    <row r="468" spans="1:4" ht="42">
       <c r="A468" t="s">
         <v>355</v>
       </c>
@@ -26545,7 +26545,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="469" spans="1:4" ht="210">
+    <row r="469" spans="1:4" ht="42">
       <c r="A469" t="s">
         <v>79</v>
       </c>
@@ -26573,7 +26573,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="471" spans="1:4" ht="112">
+    <row r="471" spans="1:4" ht="28">
       <c r="A471" t="s">
         <v>357</v>
       </c>
@@ -26587,7 +26587,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="472" spans="1:4" ht="154">
+    <row r="472" spans="1:4" ht="28">
       <c r="A472" t="s">
         <v>358</v>
       </c>
@@ -26643,7 +26643,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="476" spans="1:4" ht="409">
+    <row r="476" spans="1:4" ht="252">
       <c r="A476" t="s">
         <v>361</v>
       </c>
@@ -26699,7 +26699,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="480" spans="1:4" ht="409">
+    <row r="480" spans="1:4" ht="364">
       <c r="A480" t="s">
         <v>191</v>
       </c>

</xml_diff>

<commit_message>
New compnay matching script for Milestone2
</commit_message>
<xml_diff>
--- a/CompanyMatches.xlsx
+++ b/CompanyMatches.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
@@ -19983,14 +19983,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D47" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="31.5" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="47.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20525,7 +20524,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="336">
+    <row r="39" spans="1:4" ht="409">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -20553,7 +20552,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="336">
+    <row r="41" spans="1:4" ht="409">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -20567,7 +20566,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="42">
+    <row r="42" spans="1:4" ht="210">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -20609,7 +20608,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="42">
+    <row r="45" spans="1:4" ht="210">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -20637,7 +20636,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="28">
+    <row r="47" spans="1:4" ht="140">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -20819,7 +20818,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" ht="42">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -20959,7 +20958,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="392">
+    <row r="70" spans="1:4" ht="409">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -21015,7 +21014,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="224">
+    <row r="74" spans="1:4" ht="409">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -21127,7 +21126,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="252">
+    <row r="82" spans="1:4" ht="409">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -21169,7 +21168,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="266">
+    <row r="85" spans="1:4" ht="409">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -21211,7 +21210,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="28">
+    <row r="88" spans="1:4" ht="154">
       <c r="A88" t="s">
         <v>82</v>
       </c>
@@ -21337,7 +21336,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="84">
+    <row r="97" spans="1:4" ht="350">
       <c r="A97" t="s">
         <v>31</v>
       </c>
@@ -21365,7 +21364,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="322">
+    <row r="99" spans="1:4" ht="409">
       <c r="A99" t="s">
         <v>90</v>
       </c>
@@ -21393,7 +21392,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="112">
+    <row r="101" spans="1:4" ht="409">
       <c r="A101" t="s">
         <v>92</v>
       </c>
@@ -21519,7 +21518,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="28">
+    <row r="110" spans="1:4" ht="154">
       <c r="A110" t="s">
         <v>100</v>
       </c>
@@ -21533,7 +21532,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="322">
+    <row r="111" spans="1:4" ht="409">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -21589,7 +21588,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="182">
+    <row r="115" spans="1:4" ht="409">
       <c r="A115" t="s">
         <v>105</v>
       </c>
@@ -21603,7 +21602,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="42">
+    <row r="116" spans="1:4" ht="210">
       <c r="A116" t="s">
         <v>106</v>
       </c>
@@ -21645,7 +21644,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="252">
+    <row r="119" spans="1:4" ht="409">
       <c r="A119" t="s">
         <v>109</v>
       </c>
@@ -21659,7 +21658,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="392">
+    <row r="120" spans="1:4" ht="409">
       <c r="A120" t="s">
         <v>31</v>
       </c>
@@ -21701,7 +21700,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="70">
+    <row r="123" spans="1:4" ht="350">
       <c r="A123" t="s">
         <v>112</v>
       </c>
@@ -21715,7 +21714,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="392">
+    <row r="124" spans="1:4" ht="409">
       <c r="A124" t="s">
         <v>113</v>
       </c>
@@ -21757,7 +21756,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="42">
+    <row r="127" spans="1:4" ht="210">
       <c r="A127" t="s">
         <v>114</v>
       </c>
@@ -21785,7 +21784,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="56">
+    <row r="129" spans="1:4" ht="224">
       <c r="A129" t="s">
         <v>116</v>
       </c>
@@ -21813,7 +21812,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" ht="56">
       <c r="A131" t="s">
         <v>118</v>
       </c>
@@ -21827,7 +21826,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="28">
+    <row r="132" spans="1:4" ht="154">
       <c r="A132" t="s">
         <v>119</v>
       </c>
@@ -21841,7 +21840,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="56">
+    <row r="133" spans="1:4" ht="224">
       <c r="A133" t="s">
         <v>120</v>
       </c>
@@ -21869,7 +21868,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="252">
+    <row r="135" spans="1:4" ht="409">
       <c r="A135" t="s">
         <v>79</v>
       </c>
@@ -21897,7 +21896,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="294">
+    <row r="137" spans="1:4" ht="409">
       <c r="A137" t="s">
         <v>122</v>
       </c>
@@ -21925,7 +21924,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" ht="56">
       <c r="A139" t="s">
         <v>124</v>
       </c>
@@ -21939,7 +21938,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" ht="70">
       <c r="A140" t="s">
         <v>32</v>
       </c>
@@ -21981,7 +21980,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="336">
+    <row r="143" spans="1:4" ht="409">
       <c r="A143" t="s">
         <v>127</v>
       </c>
@@ -22009,7 +22008,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="322">
+    <row r="145" spans="1:4" ht="409">
       <c r="A145" t="s">
         <v>129</v>
       </c>
@@ -22051,7 +22050,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" ht="56">
       <c r="A148" t="s">
         <v>132</v>
       </c>
@@ -22065,7 +22064,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" ht="70">
       <c r="A149" t="s">
         <v>133</v>
       </c>
@@ -22079,7 +22078,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" ht="56">
       <c r="A150" t="s">
         <v>79</v>
       </c>
@@ -22093,7 +22092,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="42">
+    <row r="151" spans="1:4" ht="168">
       <c r="A151" t="s">
         <v>134</v>
       </c>
@@ -22149,7 +22148,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="42">
+    <row r="155" spans="1:4" ht="168">
       <c r="A155" t="s">
         <v>138</v>
       </c>
@@ -22219,7 +22218,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" ht="84">
       <c r="A160" t="s">
         <v>142</v>
       </c>
@@ -22317,7 +22316,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="322">
+    <row r="167" spans="1:4" ht="409">
       <c r="A167" t="s">
         <v>148</v>
       </c>
@@ -22373,7 +22372,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" ht="56">
       <c r="A171" t="s">
         <v>150</v>
       </c>
@@ -22415,7 +22414,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="294">
+    <row r="174" spans="1:4" ht="409">
       <c r="A174" t="s">
         <v>153</v>
       </c>
@@ -22443,7 +22442,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="336">
+    <row r="176" spans="1:4" ht="409">
       <c r="A176" t="s">
         <v>154</v>
       </c>
@@ -22471,7 +22470,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="28">
+    <row r="178" spans="1:4" ht="112">
       <c r="A178" t="s">
         <v>156</v>
       </c>
@@ -22513,7 +22512,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="42">
+    <row r="181" spans="1:4" ht="210">
       <c r="A181" t="s">
         <v>158</v>
       </c>
@@ -22527,7 +22526,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="126">
+    <row r="182" spans="1:4" ht="409">
       <c r="A182" t="s">
         <v>33</v>
       </c>
@@ -22583,7 +22582,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="322">
+    <row r="186" spans="1:4" ht="409">
       <c r="A186" t="s">
         <v>161</v>
       </c>
@@ -22597,7 +22596,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="378">
+    <row r="187" spans="1:4" ht="409">
       <c r="A187" t="s">
         <v>84</v>
       </c>
@@ -22625,7 +22624,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="28">
+    <row r="189" spans="1:4" ht="154">
       <c r="A189" t="s">
         <v>163</v>
       </c>
@@ -22681,7 +22680,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="238">
+    <row r="193" spans="1:4" ht="409">
       <c r="A193" t="s">
         <v>89</v>
       </c>
@@ -22723,7 +22722,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="42">
+    <row r="196" spans="1:4" ht="210">
       <c r="A196" t="s">
         <v>168</v>
       </c>
@@ -22793,7 +22792,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="308">
+    <row r="201" spans="1:4" ht="409">
       <c r="A201" t="s">
         <v>171</v>
       </c>
@@ -22821,7 +22820,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="182">
+    <row r="203" spans="1:4" ht="409">
       <c r="A203" t="s">
         <v>173</v>
       </c>
@@ -22919,7 +22918,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="154">
+    <row r="210" spans="1:4" ht="409">
       <c r="A210" t="s">
         <v>178</v>
       </c>
@@ -23045,7 +23044,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="322">
+    <row r="219" spans="1:4" ht="409">
       <c r="A219" t="s">
         <v>5</v>
       </c>
@@ -23101,7 +23100,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="168">
+    <row r="223" spans="1:4" ht="409">
       <c r="A223" t="s">
         <v>189</v>
       </c>
@@ -23143,7 +23142,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="226" spans="1:4">
+    <row r="226" spans="1:4" ht="56">
       <c r="A226" t="s">
         <v>192</v>
       </c>
@@ -23213,7 +23212,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="231" spans="1:4">
+    <row r="231" spans="1:4" ht="56">
       <c r="A231" t="s">
         <v>81</v>
       </c>
@@ -23255,7 +23254,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="28">
+    <row r="234" spans="1:4" ht="154">
       <c r="A234" t="s">
         <v>196</v>
       </c>
@@ -23311,7 +23310,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="238" spans="1:4">
+    <row r="238" spans="1:4" ht="42">
       <c r="A238" t="s">
         <v>59</v>
       </c>
@@ -23339,7 +23338,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="240" spans="1:4">
+    <row r="240" spans="1:4" ht="56">
       <c r="A240" t="s">
         <v>201</v>
       </c>
@@ -23381,7 +23380,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="28">
+    <row r="243" spans="1:4" ht="154">
       <c r="A243" t="s">
         <v>203</v>
       </c>
@@ -23437,7 +23436,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="42">
+    <row r="247" spans="1:4" ht="210">
       <c r="A247" t="s">
         <v>205</v>
       </c>
@@ -23451,7 +23450,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="280">
+    <row r="248" spans="1:4" ht="409">
       <c r="A248" t="s">
         <v>206</v>
       </c>
@@ -23479,7 +23478,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="42">
+    <row r="250" spans="1:4" ht="210">
       <c r="A250" t="s">
         <v>208</v>
       </c>
@@ -23703,7 +23702,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="42">
+    <row r="266" spans="1:4" ht="210">
       <c r="A266" t="s">
         <v>42</v>
       </c>
@@ -23801,7 +23800,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="42">
+    <row r="273" spans="1:4" ht="210">
       <c r="A273" t="s">
         <v>225</v>
       </c>
@@ -23815,7 +23814,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="28">
+    <row r="274" spans="1:4" ht="154">
       <c r="A274" t="s">
         <v>226</v>
       </c>
@@ -23829,7 +23828,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="98">
+    <row r="275" spans="1:4" ht="409">
       <c r="A275" t="s">
         <v>5</v>
       </c>
@@ -23857,7 +23856,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="112">
+    <row r="277" spans="1:4" ht="409">
       <c r="A277" t="s">
         <v>228</v>
       </c>
@@ -23899,7 +23898,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="350">
+    <row r="280" spans="1:4" ht="409">
       <c r="A280" t="s">
         <v>230</v>
       </c>
@@ -23969,7 +23968,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="336">
+    <row r="285" spans="1:4" ht="409">
       <c r="A285" t="s">
         <v>65</v>
       </c>
@@ -23997,7 +23996,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="140">
+    <row r="287" spans="1:4" ht="409">
       <c r="A287" t="s">
         <v>235</v>
       </c>
@@ -24025,7 +24024,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="289" spans="1:4">
+    <row r="289" spans="1:4" ht="70">
       <c r="A289" t="s">
         <v>237</v>
       </c>
@@ -24081,7 +24080,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="28">
+    <row r="293" spans="1:4" ht="126">
       <c r="A293" t="s">
         <v>241</v>
       </c>
@@ -24109,7 +24108,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="42">
+    <row r="295" spans="1:4" ht="210">
       <c r="A295" t="s">
         <v>243</v>
       </c>
@@ -24137,7 +24136,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="336">
+    <row r="297" spans="1:4" ht="409">
       <c r="A297" t="s">
         <v>245</v>
       </c>
@@ -24165,7 +24164,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="70">
+    <row r="299" spans="1:4" ht="266">
       <c r="A299" t="s">
         <v>247</v>
       </c>
@@ -24235,7 +24234,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="304" spans="1:4" ht="322">
+    <row r="304" spans="1:4" ht="409">
       <c r="A304" t="s">
         <v>191</v>
       </c>
@@ -24249,7 +24248,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="392">
+    <row r="305" spans="1:4" ht="409">
       <c r="A305" t="s">
         <v>251</v>
       </c>
@@ -24319,7 +24318,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="252">
+    <row r="310" spans="1:4" ht="409">
       <c r="A310" t="s">
         <v>207</v>
       </c>
@@ -24347,7 +24346,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="28">
+    <row r="312" spans="1:4" ht="112">
       <c r="A312" t="s">
         <v>257</v>
       </c>
@@ -24375,7 +24374,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="314" spans="1:4">
+    <row r="314" spans="1:4" ht="56">
       <c r="A314" t="s">
         <v>258</v>
       </c>
@@ -24403,7 +24402,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="42">
+    <row r="316" spans="1:4" ht="210">
       <c r="A316" t="s">
         <v>107</v>
       </c>
@@ -24473,7 +24472,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="321" spans="1:4" ht="350">
+    <row r="321" spans="1:4" ht="409">
       <c r="A321" t="s">
         <v>24</v>
       </c>
@@ -24515,7 +24514,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="324" spans="1:4" ht="84">
+    <row r="324" spans="1:4" ht="409">
       <c r="A324" t="s">
         <v>264</v>
       </c>
@@ -24557,7 +24556,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="327" spans="1:4" ht="28">
+    <row r="327" spans="1:4" ht="154">
       <c r="A327" t="s">
         <v>59</v>
       </c>
@@ -24669,7 +24668,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="335" spans="1:4" ht="42">
+    <row r="335" spans="1:4" ht="210">
       <c r="A335" t="s">
         <v>271</v>
       </c>
@@ -24711,7 +24710,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="338" spans="1:4" ht="28">
+    <row r="338" spans="1:4" ht="140">
       <c r="A338" t="s">
         <v>273</v>
       </c>
@@ -24725,7 +24724,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="339" spans="1:4">
+    <row r="339" spans="1:4" ht="56">
       <c r="A339" t="s">
         <v>274</v>
       </c>
@@ -24739,7 +24738,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="340" spans="1:4" ht="42">
+    <row r="340" spans="1:4" ht="210">
       <c r="A340" t="s">
         <v>89</v>
       </c>
@@ -24767,7 +24766,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="342" spans="1:4">
+    <row r="342" spans="1:4" ht="56">
       <c r="A342" t="s">
         <v>276</v>
       </c>
@@ -24851,7 +24850,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="348" spans="1:4" ht="28">
+    <row r="348" spans="1:4" ht="154">
       <c r="A348" t="s">
         <v>40</v>
       </c>
@@ -24921,7 +24920,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="353" spans="1:4" ht="28">
+    <row r="353" spans="1:4" ht="154">
       <c r="A353" t="s">
         <v>284</v>
       </c>
@@ -24963,7 +24962,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="356" spans="1:4">
+    <row r="356" spans="1:4" ht="70">
       <c r="A356" t="s">
         <v>35</v>
       </c>
@@ -24991,7 +24990,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="358" spans="1:4" ht="98">
+    <row r="358" spans="1:4" ht="409">
       <c r="A358" t="s">
         <v>286</v>
       </c>
@@ -25005,7 +25004,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="359" spans="1:4">
+    <row r="359" spans="1:4" ht="42">
       <c r="A359" t="s">
         <v>287</v>
       </c>
@@ -25019,7 +25018,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="360" spans="1:4" ht="42">
+    <row r="360" spans="1:4" ht="210">
       <c r="A360" t="s">
         <v>288</v>
       </c>
@@ -25033,7 +25032,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="361" spans="1:4" ht="56">
+    <row r="361" spans="1:4" ht="238">
       <c r="A361" t="s">
         <v>289</v>
       </c>
@@ -25145,7 +25144,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="369" spans="1:4" ht="252">
+    <row r="369" spans="1:4" ht="409">
       <c r="A369" t="s">
         <v>295</v>
       </c>
@@ -25187,7 +25186,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="372" spans="1:4" ht="266">
+    <row r="372" spans="1:4" ht="409">
       <c r="A372" t="s">
         <v>107</v>
       </c>
@@ -25285,7 +25284,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="379" spans="1:4" ht="42">
+    <row r="379" spans="1:4" ht="210">
       <c r="A379" t="s">
         <v>303</v>
       </c>
@@ -25313,7 +25312,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="381" spans="1:4" ht="70">
+    <row r="381" spans="1:4" ht="392">
       <c r="A381" t="s">
         <v>305</v>
       </c>
@@ -25383,7 +25382,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="386" spans="1:4">
+    <row r="386" spans="1:4" ht="56">
       <c r="A386" t="s">
         <v>309</v>
       </c>
@@ -25397,7 +25396,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="387" spans="1:4" ht="210">
+    <row r="387" spans="1:4" ht="409">
       <c r="A387" t="s">
         <v>89</v>
       </c>
@@ -25411,7 +25410,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="388" spans="1:4">
+    <row r="388" spans="1:4" ht="70">
       <c r="A388" t="s">
         <v>35</v>
       </c>
@@ -25425,7 +25424,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="389" spans="1:4" ht="70">
+    <row r="389" spans="1:4" ht="392">
       <c r="A389" t="s">
         <v>310</v>
       </c>
@@ -25677,7 +25676,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="407" spans="1:4" ht="28">
+    <row r="407" spans="1:4" ht="154">
       <c r="A407" t="s">
         <v>321</v>
       </c>
@@ -25691,7 +25690,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="408" spans="1:4" ht="28">
+    <row r="408" spans="1:4" ht="154">
       <c r="A408" t="s">
         <v>322</v>
       </c>
@@ -25719,7 +25718,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="410" spans="1:4" ht="28">
+    <row r="410" spans="1:4" ht="154">
       <c r="A410" t="s">
         <v>323</v>
       </c>
@@ -25803,7 +25802,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="416" spans="1:4" ht="56">
+    <row r="416" spans="1:4" ht="224">
       <c r="A416" t="s">
         <v>227</v>
       </c>
@@ -25817,7 +25816,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="417" spans="1:4" ht="364">
+    <row r="417" spans="1:4" ht="409">
       <c r="A417" t="s">
         <v>326</v>
       </c>
@@ -25831,7 +25830,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="418" spans="1:4" ht="56">
+    <row r="418" spans="1:4" ht="266">
       <c r="A418" t="s">
         <v>327</v>
       </c>
@@ -25845,7 +25844,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="419" spans="1:4" ht="308">
+    <row r="419" spans="1:4" ht="409">
       <c r="A419" t="s">
         <v>84</v>
       </c>
@@ -25873,7 +25872,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="421" spans="1:4" ht="322">
+    <row r="421" spans="1:4" ht="409">
       <c r="A421" t="s">
         <v>328</v>
       </c>
@@ -25887,7 +25886,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="422" spans="1:4" ht="182">
+    <row r="422" spans="1:4" ht="409">
       <c r="A422" t="s">
         <v>118</v>
       </c>
@@ -25957,7 +25956,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="427" spans="1:4" ht="28">
+    <row r="427" spans="1:4" ht="154">
       <c r="A427" t="s">
         <v>306</v>
       </c>
@@ -25985,7 +25984,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="429" spans="1:4" ht="406">
+    <row r="429" spans="1:4" ht="409">
       <c r="A429" t="s">
         <v>334</v>
       </c>
@@ -26013,7 +26012,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="431" spans="1:4" ht="42">
+    <row r="431" spans="1:4" ht="210">
       <c r="A431" t="s">
         <v>335</v>
       </c>
@@ -26041,7 +26040,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="433" spans="1:4" ht="56">
+    <row r="433" spans="1:4" ht="224">
       <c r="A433" t="s">
         <v>336</v>
       </c>
@@ -26069,7 +26068,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="435" spans="1:4">
+    <row r="435" spans="1:4" ht="42">
       <c r="A435" t="s">
         <v>45</v>
       </c>
@@ -26083,7 +26082,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="436" spans="1:4" ht="84">
+    <row r="436" spans="1:4" ht="409">
       <c r="A436" t="s">
         <v>337</v>
       </c>
@@ -26139,7 +26138,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="440" spans="1:4" ht="364">
+    <row r="440" spans="1:4" ht="409">
       <c r="A440" t="s">
         <v>339</v>
       </c>
@@ -26153,7 +26152,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="441" spans="1:4" ht="70">
+    <row r="441" spans="1:4" ht="392">
       <c r="A441" t="s">
         <v>13</v>
       </c>
@@ -26209,7 +26208,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="445" spans="1:4" ht="42">
+    <row r="445" spans="1:4" ht="210">
       <c r="A445" t="s">
         <v>342</v>
       </c>
@@ -26251,7 +26250,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="448" spans="1:4" ht="238">
+    <row r="448" spans="1:4" ht="409">
       <c r="A448" t="s">
         <v>84</v>
       </c>
@@ -26279,7 +26278,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="450" spans="1:4" ht="84">
+    <row r="450" spans="1:4" ht="409">
       <c r="A450" t="s">
         <v>344</v>
       </c>
@@ -26293,7 +26292,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="451" spans="1:4" ht="308">
+    <row r="451" spans="1:4" ht="409">
       <c r="A451" t="s">
         <v>345</v>
       </c>
@@ -26475,7 +26474,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="464" spans="1:4">
+    <row r="464" spans="1:4" ht="70">
       <c r="A464" t="s">
         <v>79</v>
       </c>
@@ -26503,7 +26502,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="466" spans="1:4" ht="84">
+    <row r="466" spans="1:4" ht="409">
       <c r="A466" t="s">
         <v>353</v>
       </c>
@@ -26517,7 +26516,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="467" spans="1:4">
+    <row r="467" spans="1:4" ht="42">
       <c r="A467" t="s">
         <v>354</v>
       </c>
@@ -26531,7 +26530,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="468" spans="1:4" ht="42">
+    <row r="468" spans="1:4" ht="210">
       <c r="A468" t="s">
         <v>355</v>
       </c>
@@ -26545,7 +26544,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="469" spans="1:4" ht="42">
+    <row r="469" spans="1:4" ht="210">
       <c r="A469" t="s">
         <v>79</v>
       </c>
@@ -26573,7 +26572,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="471" spans="1:4" ht="28">
+    <row r="471" spans="1:4" ht="112">
       <c r="A471" t="s">
         <v>357</v>
       </c>
@@ -26587,7 +26586,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="472" spans="1:4" ht="28">
+    <row r="472" spans="1:4" ht="154">
       <c r="A472" t="s">
         <v>358</v>
       </c>
@@ -26643,7 +26642,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="476" spans="1:4" ht="252">
+    <row r="476" spans="1:4" ht="409">
       <c r="A476" t="s">
         <v>361</v>
       </c>
@@ -26699,7 +26698,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="480" spans="1:4" ht="364">
+    <row r="480" spans="1:4" ht="409">
       <c r="A480" t="s">
         <v>191</v>
       </c>

</xml_diff>